<commit_message>
clean remarks and remarks definitions
</commit_message>
<xml_diff>
--- a/ETL/FAA-Airports-data/airport-data-dictionaries.xlsx
+++ b/ETL/FAA-Airports-data/airport-data-dictionaries.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Inetpub\wwwroot\Development\webcont\airports\airport_safety\airportdata_5010\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpatterson/Desktop/Analytics-Coding/Projects/US-Airports/ETL/FAA-Airports-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CD29B7-53F8-CE43-AB16-B5746E78E5CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="9570" windowHeight="9420"/>
+    <workbookView xWindow="28860" yWindow="2380" windowWidth="19560" windowHeight="14900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Facilities" sheetId="1" r:id="rId1"/>
@@ -28,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Crader, Mike CTR (FAA)</author>
   </authors>
   <commentList>
-    <comment ref="A104" authorId="0" shapeId="0">
+    <comment ref="A104" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1744,8 +1745,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1964,9 +1965,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Remarks" xfId="1"/>
-    <cellStyle name="Normal_Runways" xfId="2"/>
-    <cellStyle name="Normal_Sheet1" xfId="3"/>
+    <cellStyle name="Normal_Remarks" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_Runways" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_Sheet1" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2057,6 +2058,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2092,6 +2110,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2267,25 +2302,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor indexed="57"/>
   </sheetPr>
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>291</v>
       </c>
@@ -2296,7 +2331,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="42">
       <c r="A2" s="7" t="s">
         <v>304</v>
       </c>
@@ -2307,7 +2342,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="28">
       <c r="A3" s="7" t="s">
         <v>306</v>
       </c>
@@ -2318,7 +2353,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="42">
       <c r="A4" s="7" t="s">
         <v>308</v>
       </c>
@@ -2329,7 +2364,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="42">
       <c r="A5" s="7" t="s">
         <v>310</v>
       </c>
@@ -2340,7 +2375,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="56">
       <c r="A6" s="7" t="s">
         <v>312</v>
       </c>
@@ -2351,7 +2386,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="14">
       <c r="A7" s="7" t="s">
         <v>314</v>
       </c>
@@ -2362,7 +2397,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="28">
       <c r="A8" s="7" t="s">
         <v>316</v>
       </c>
@@ -2373,7 +2408,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="14">
       <c r="A9" s="7" t="s">
         <v>318</v>
       </c>
@@ -2384,7 +2419,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="14">
       <c r="A10" s="7" t="s">
         <v>320</v>
       </c>
@@ -2395,7 +2430,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="42">
       <c r="A11" s="7" t="s">
         <v>322</v>
       </c>
@@ -2406,7 +2441,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="14">
       <c r="A12" s="7" t="s">
         <v>324</v>
       </c>
@@ -2417,7 +2452,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="14">
       <c r="A13" s="7" t="s">
         <v>326</v>
       </c>
@@ -2428,7 +2463,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="42">
       <c r="A14" s="7" t="s">
         <v>328</v>
       </c>
@@ -2439,7 +2474,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="14">
       <c r="A15" s="7" t="s">
         <v>330</v>
       </c>
@@ -2450,7 +2485,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="14">
       <c r="A16" s="7" t="s">
         <v>332</v>
       </c>
@@ -2461,7 +2496,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="14">
       <c r="A17" s="7" t="s">
         <v>334</v>
       </c>
@@ -2472,7 +2507,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="14">
       <c r="A18" s="7" t="s">
         <v>336</v>
       </c>
@@ -2483,7 +2518,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="42">
       <c r="A19" s="7" t="s">
         <v>338</v>
       </c>
@@ -2494,7 +2529,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="14">
       <c r="A20" s="7" t="s">
         <v>339</v>
       </c>
@@ -2505,7 +2540,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="14">
       <c r="A21" s="7" t="s">
         <v>341</v>
       </c>
@@ -2516,7 +2551,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="14">
       <c r="A22" s="7" t="s">
         <v>343</v>
       </c>
@@ -2527,7 +2562,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="42">
       <c r="A23" s="7" t="s">
         <v>345</v>
       </c>
@@ -2538,7 +2573,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="14">
       <c r="A24" s="7" t="s">
         <v>346</v>
       </c>
@@ -2549,7 +2584,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="14">
       <c r="A25" s="7" t="s">
         <v>348</v>
       </c>
@@ -2560,7 +2595,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="14">
       <c r="A26" s="7" t="s">
         <v>350</v>
       </c>
@@ -2571,7 +2606,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="14">
       <c r="A27" s="7" t="s">
         <v>352</v>
       </c>
@@ -2582,7 +2617,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="28">
       <c r="A28" s="7" t="s">
         <v>354</v>
       </c>
@@ -2593,7 +2628,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="56">
       <c r="A29" s="7" t="s">
         <v>356</v>
       </c>
@@ -2604,7 +2639,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="28">
       <c r="A30" s="7" t="s">
         <v>358</v>
       </c>
@@ -2615,7 +2650,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="28">
       <c r="A31" s="7" t="s">
         <v>361</v>
       </c>
@@ -2626,7 +2661,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="14">
       <c r="A32" s="7" t="s">
         <v>363</v>
       </c>
@@ -2637,7 +2672,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="14">
       <c r="A33" s="7" t="s">
         <v>365</v>
       </c>
@@ -2648,7 +2683,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="28">
       <c r="A34" s="7" t="s">
         <v>367</v>
       </c>
@@ -2659,7 +2694,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="28">
       <c r="A35" s="7" t="s">
         <v>369</v>
       </c>
@@ -2670,7 +2705,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="28">
       <c r="A36" s="7" t="s">
         <v>371</v>
       </c>
@@ -2681,7 +2716,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="14">
       <c r="A37" s="7" t="s">
         <v>474</v>
       </c>
@@ -2692,7 +2727,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="84">
       <c r="A38" s="7" t="s">
         <v>373</v>
       </c>
@@ -2703,7 +2738,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="28">
       <c r="A39" s="7" t="s">
         <v>374</v>
       </c>
@@ -2714,7 +2749,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="14">
       <c r="A40" s="7" t="s">
         <v>376</v>
       </c>
@@ -2725,7 +2760,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="56">
       <c r="A41" s="7" t="s">
         <v>378</v>
       </c>
@@ -2736,7 +2771,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="28">
       <c r="A42" s="7" t="s">
         <v>380</v>
       </c>
@@ -2747,7 +2782,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="14">
       <c r="A43" s="7" t="s">
         <v>382</v>
       </c>
@@ -2758,7 +2793,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="28">
       <c r="A44" s="7" t="s">
         <v>384</v>
       </c>
@@ -2769,7 +2804,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="28">
       <c r="A45" s="7" t="s">
         <v>386</v>
       </c>
@@ -2780,7 +2815,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="14">
       <c r="A46" s="7" t="s">
         <v>388</v>
       </c>
@@ -2791,7 +2826,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="28">
       <c r="A47" s="7" t="s">
         <v>475</v>
       </c>
@@ -2802,7 +2837,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="196">
       <c r="A48" s="7" t="s">
         <v>390</v>
       </c>
@@ -2813,7 +2848,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="56">
       <c r="A49" s="7" t="s">
         <v>391</v>
       </c>
@@ -2824,7 +2859,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="28">
       <c r="A50" s="7" t="s">
         <v>393</v>
       </c>
@@ -2835,7 +2870,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="191.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="196">
       <c r="A51" s="7" t="s">
         <v>395</v>
       </c>
@@ -2846,7 +2881,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="42">
       <c r="A52" s="7" t="s">
         <v>396</v>
       </c>
@@ -2857,7 +2892,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="28">
       <c r="A53" s="7" t="s">
         <v>398</v>
       </c>
@@ -2868,7 +2903,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="56">
       <c r="A54" s="7" t="s">
         <v>400</v>
       </c>
@@ -2879,7 +2914,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="28">
       <c r="A55" s="7" t="s">
         <v>476</v>
       </c>
@@ -2890,7 +2925,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="204" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="196">
       <c r="A56" s="7" t="s">
         <v>402</v>
       </c>
@@ -2901,7 +2936,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="252">
       <c r="A57" s="7" t="s">
         <v>403</v>
       </c>
@@ -2912,7 +2947,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="42">
       <c r="A58" s="7" t="s">
         <v>404</v>
       </c>
@@ -2923,7 +2958,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="42">
       <c r="A59" s="7" t="s">
         <v>406</v>
       </c>
@@ -2934,7 +2969,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="28">
       <c r="A60" s="7" t="s">
         <v>408</v>
       </c>
@@ -2945,7 +2980,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="42">
       <c r="A61" s="7" t="s">
         <v>410</v>
       </c>
@@ -2956,7 +2991,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="28">
       <c r="A62" s="7" t="s">
         <v>412</v>
       </c>
@@ -2967,7 +3002,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="42">
       <c r="A63" s="7" t="s">
         <v>414</v>
       </c>
@@ -2978,7 +3013,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="42">
       <c r="A64" s="7" t="s">
         <v>416</v>
       </c>
@@ -2989,7 +3024,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="14">
       <c r="A65" s="7" t="s">
         <v>418</v>
       </c>
@@ -3000,7 +3035,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="28">
       <c r="A66" s="7" t="s">
         <v>420</v>
       </c>
@@ -3011,7 +3046,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="154">
       <c r="A67" s="7" t="s">
         <v>422</v>
       </c>
@@ -3022,7 +3057,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="28">
       <c r="A68" s="7" t="s">
         <v>423</v>
       </c>
@@ -3033,7 +3068,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="28">
       <c r="A69" s="7" t="s">
         <v>425</v>
       </c>
@@ -3044,7 +3079,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="42">
       <c r="A70" s="7" t="s">
         <v>427</v>
       </c>
@@ -3055,7 +3090,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="42">
       <c r="A71" s="7" t="s">
         <v>429</v>
       </c>
@@ -3066,7 +3101,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="42">
       <c r="A72" s="7" t="s">
         <v>436</v>
       </c>
@@ -3077,7 +3112,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="70">
       <c r="A73" s="7" t="s">
         <v>554</v>
       </c>
@@ -3088,7 +3123,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="28">
       <c r="A74" s="7" t="s">
         <v>438</v>
       </c>
@@ -3099,7 +3134,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="42">
       <c r="A75" s="7" t="s">
         <v>440</v>
       </c>
@@ -3110,7 +3145,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="14">
       <c r="A76" s="7" t="s">
         <v>442</v>
       </c>
@@ -3121,7 +3156,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="28">
       <c r="A77" s="7" t="s">
         <v>446</v>
       </c>
@@ -3132,7 +3167,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="70">
       <c r="A78" s="7" t="s">
         <v>448</v>
       </c>
@@ -3143,7 +3178,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="28">
       <c r="A79" s="7" t="s">
         <v>450</v>
       </c>
@@ -3154,7 +3189,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="28">
       <c r="A80" s="7" t="s">
         <v>12</v>
       </c>
@@ -3165,7 +3200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="14">
       <c r="A81" s="7" t="s">
         <v>452</v>
       </c>
@@ -3176,7 +3211,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="14">
       <c r="A82" s="7" t="s">
         <v>454</v>
       </c>
@@ -3187,7 +3222,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="14">
       <c r="A83" s="7" t="s">
         <v>456</v>
       </c>
@@ -3198,7 +3233,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="14">
       <c r="A84" s="7" t="s">
         <v>458</v>
       </c>
@@ -3209,7 +3244,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="14">
       <c r="A85" s="7" t="s">
         <v>460</v>
       </c>
@@ -3220,7 +3255,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="14">
       <c r="A86" s="7" t="s">
         <v>462</v>
       </c>
@@ -3231,7 +3266,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="14">
       <c r="A87" s="7" t="s">
         <v>464</v>
       </c>
@@ -3242,7 +3277,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="28">
       <c r="A88" s="7" t="s">
         <v>477</v>
       </c>
@@ -3253,7 +3288,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="28">
       <c r="A89" s="7" t="s">
         <v>293</v>
       </c>
@@ -3264,7 +3299,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="28">
       <c r="A90" s="7" t="s">
         <v>466</v>
       </c>
@@ -3275,7 +3310,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="28">
       <c r="A91" s="7" t="s">
         <v>468</v>
       </c>
@@ -3286,7 +3321,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="42">
       <c r="A92" s="7" t="s">
         <v>470</v>
       </c>
@@ -3297,7 +3332,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="14">
       <c r="A93" s="7" t="s">
         <v>472</v>
       </c>
@@ -3308,7 +3343,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="28">
       <c r="A94" s="8" t="s">
         <v>478</v>
       </c>
@@ -3319,7 +3354,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="14">
       <c r="A95" s="7" t="s">
         <v>294</v>
       </c>
@@ -3330,7 +3365,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="14">
       <c r="A96" s="7" t="s">
         <v>296</v>
       </c>
@@ -3341,7 +3376,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="14">
       <c r="A97" s="7" t="s">
         <v>298</v>
       </c>
@@ -3352,7 +3387,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="14">
       <c r="A98" s="7" t="s">
         <v>300</v>
       </c>
@@ -3363,7 +3398,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="14">
       <c r="A99" s="7" t="s">
         <v>302</v>
       </c>
@@ -3374,7 +3409,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="14">
       <c r="A100" s="7" t="s">
         <v>431</v>
       </c>
@@ -3385,7 +3420,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="14">
       <c r="A101" s="7" t="s">
         <v>433</v>
       </c>
@@ -3396,7 +3431,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="14">
       <c r="A102" s="7" t="s">
         <v>444</v>
       </c>
@@ -3407,7 +3442,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="14">
       <c r="A103" s="8" t="s">
         <v>42</v>
       </c>
@@ -3418,7 +3453,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="14">
       <c r="A104" s="12" t="s">
         <v>557</v>
       </c>
@@ -3439,25 +3474,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor indexed="57"/>
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>291</v>
       </c>
@@ -3468,7 +3503,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="56">
       <c r="A2" s="6" t="s">
         <v>304</v>
       </c>
@@ -3479,7 +3514,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="42">
       <c r="A3" s="6" t="s">
         <v>316</v>
       </c>
@@ -3490,7 +3525,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="112">
       <c r="A4" s="6" t="s">
         <v>491</v>
       </c>
@@ -3501,7 +3536,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="28">
       <c r="A5" s="6" t="s">
         <v>492</v>
       </c>
@@ -3520,26 +3555,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor indexed="57"/>
   </sheetPr>
   <dimension ref="A1:C134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A2" sqref="A1:IV65536"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51:IV51"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>291</v>
       </c>
@@ -3550,7 +3585,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="56">
       <c r="A2" s="5" t="s">
         <v>304</v>
       </c>
@@ -3561,7 +3596,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="42">
       <c r="A3" s="5" t="s">
         <v>316</v>
       </c>
@@ -3572,7 +3607,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="42">
       <c r="A4" s="5" t="s">
         <v>109</v>
       </c>
@@ -3583,7 +3618,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="14">
       <c r="A5" s="5" t="s">
         <v>111</v>
       </c>
@@ -3594,7 +3629,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="14">
       <c r="A6" s="5" t="s">
         <v>120</v>
       </c>
@@ -3605,7 +3640,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="112">
       <c r="A7" s="5" t="s">
         <v>119</v>
       </c>
@@ -3616,7 +3651,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="56">
       <c r="A8" s="5" t="s">
         <v>117</v>
       </c>
@@ -3627,7 +3662,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="70">
       <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
@@ -3638,7 +3673,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="42">
       <c r="A10" s="5" t="s">
         <v>45</v>
       </c>
@@ -3649,7 +3684,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="42">
       <c r="A11" s="5" t="s">
         <v>533</v>
       </c>
@@ -3660,7 +3695,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="42">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
@@ -3671,7 +3706,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="70">
       <c r="A13" s="5" t="s">
         <v>535</v>
       </c>
@@ -3682,7 +3717,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="28">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -3693,7 +3728,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="70">
       <c r="A15" s="5" t="s">
         <v>541</v>
       </c>
@@ -3704,7 +3739,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="14">
       <c r="A16" s="5" t="s">
         <v>539</v>
       </c>
@@ -3715,7 +3750,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="14">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -3726,7 +3761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="14">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -3737,7 +3772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="14">
       <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
@@ -3748,7 +3783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="14">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -3759,7 +3794,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="28">
       <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
@@ -3770,7 +3805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="42">
       <c r="A22" s="5" t="s">
         <v>501</v>
       </c>
@@ -3781,7 +3816,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="14">
       <c r="A23" s="5" t="s">
         <v>527</v>
       </c>
@@ -3792,7 +3827,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="14">
       <c r="A24" s="5" t="s">
         <v>505</v>
       </c>
@@ -3803,7 +3838,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="14">
       <c r="A25" s="5" t="s">
         <v>507</v>
       </c>
@@ -3814,7 +3849,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="14">
       <c r="A26" s="5" t="s">
         <v>511</v>
       </c>
@@ -3825,7 +3860,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="14">
       <c r="A27" s="5" t="s">
         <v>513</v>
       </c>
@@ -3836,7 +3871,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="28">
       <c r="A28" s="5" t="s">
         <v>503</v>
       </c>
@@ -3847,7 +3882,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="28">
       <c r="A29" s="5" t="s">
         <v>509</v>
       </c>
@@ -3858,7 +3893,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="14">
       <c r="A30" s="5" t="s">
         <v>31</v>
       </c>
@@ -3869,7 +3904,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="70">
       <c r="A31" s="5" t="s">
         <v>41</v>
       </c>
@@ -3880,7 +3915,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="70">
       <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
@@ -3891,7 +3926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="28">
       <c r="A33" s="5" t="s">
         <v>25</v>
       </c>
@@ -3902,7 +3937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="70">
       <c r="A34" s="5" t="s">
         <v>497</v>
       </c>
@@ -3913,7 +3948,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="28">
       <c r="A35" s="5" t="s">
         <v>19</v>
       </c>
@@ -3924,7 +3959,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="14">
       <c r="A36" s="5" t="s">
         <v>499</v>
       </c>
@@ -3935,7 +3970,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="28">
       <c r="A37" s="5" t="s">
         <v>33</v>
       </c>
@@ -3946,7 +3981,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="14">
       <c r="A38" s="5" t="s">
         <v>545</v>
       </c>
@@ -3957,7 +3992,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="28">
       <c r="A39" s="5" t="s">
         <v>551</v>
       </c>
@@ -3968,7 +4003,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="70">
       <c r="A40" s="5" t="s">
         <v>1</v>
       </c>
@@ -3979,7 +4014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="56">
       <c r="A41" s="5" t="s">
         <v>543</v>
       </c>
@@ -3990,7 +4025,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="28">
       <c r="A42" s="5" t="s">
         <v>549</v>
       </c>
@@ -4001,7 +4036,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="56">
       <c r="A43" s="5" t="s">
         <v>547</v>
       </c>
@@ -4012,7 +4047,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="70">
       <c r="A44" s="5" t="s">
         <v>553</v>
       </c>
@@ -4023,7 +4058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="42">
       <c r="A45" s="5" t="s">
         <v>73</v>
       </c>
@@ -4034,7 +4069,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="42">
       <c r="A46" s="5" t="s">
         <v>106</v>
       </c>
@@ -4045,7 +4080,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="70">
       <c r="A47" s="5" t="s">
         <v>76</v>
       </c>
@@ -4056,7 +4091,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="28">
       <c r="A48" s="5" t="s">
         <v>97</v>
       </c>
@@ -4067,7 +4102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="70">
       <c r="A49" s="5" t="s">
         <v>79</v>
       </c>
@@ -4078,7 +4113,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="14">
       <c r="A50" s="5" t="s">
         <v>78</v>
       </c>
@@ -4089,7 +4124,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="14">
       <c r="A51" s="5" t="s">
         <v>90</v>
       </c>
@@ -4100,7 +4135,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="14">
       <c r="A52" s="5" t="s">
         <v>91</v>
       </c>
@@ -4111,7 +4146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="14">
       <c r="A53" s="5" t="s">
         <v>92</v>
       </c>
@@ -4122,7 +4157,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="28">
       <c r="A54" s="5" t="s">
         <v>93</v>
       </c>
@@ -4133,7 +4168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="28">
       <c r="A55" s="5" t="s">
         <v>89</v>
       </c>
@@ -4144,7 +4179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="42">
       <c r="A56" s="5" t="s">
         <v>56</v>
       </c>
@@ -4155,7 +4190,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="14">
       <c r="A57" s="5" t="s">
         <v>70</v>
       </c>
@@ -4166,7 +4201,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="14">
       <c r="A58" s="5" t="s">
         <v>59</v>
       </c>
@@ -4177,7 +4212,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="14">
       <c r="A59" s="5" t="s">
         <v>60</v>
       </c>
@@ -4188,7 +4223,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="28">
       <c r="A60" s="5" t="s">
         <v>62</v>
       </c>
@@ -4199,7 +4234,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="28">
       <c r="A61" s="5" t="s">
         <v>63</v>
       </c>
@@ -4210,7 +4245,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="28">
       <c r="A62" s="5" t="s">
         <v>57</v>
       </c>
@@ -4221,7 +4256,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="28">
       <c r="A63" s="5" t="s">
         <v>61</v>
       </c>
@@ -4232,7 +4267,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="14">
       <c r="A64" s="5" t="s">
         <v>102</v>
       </c>
@@ -4243,7 +4278,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="70">
       <c r="A65" s="5" t="s">
         <v>108</v>
       </c>
@@ -4254,7 +4289,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="70">
       <c r="A66" s="5" t="s">
         <v>98</v>
       </c>
@@ -4265,7 +4300,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="28">
       <c r="A67" s="5" t="s">
         <v>99</v>
       </c>
@@ -4276,7 +4311,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="70">
       <c r="A68" s="5" t="s">
         <v>54</v>
       </c>
@@ -4287,7 +4322,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="28">
       <c r="A69" s="5" t="s">
         <v>96</v>
       </c>
@@ -4298,7 +4333,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="14">
       <c r="A70" s="5" t="s">
         <v>55</v>
       </c>
@@ -4309,7 +4344,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="28">
       <c r="A71" s="5" t="s">
         <v>103</v>
       </c>
@@ -4320,7 +4355,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="14">
       <c r="A72" s="5" t="s">
         <v>81</v>
       </c>
@@ -4331,7 +4366,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="28">
       <c r="A73" s="5" t="s">
         <v>86</v>
       </c>
@@ -4342,7 +4377,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="70">
       <c r="A74" s="5" t="s">
         <v>88</v>
       </c>
@@ -4353,7 +4388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="56">
       <c r="A75" s="5" t="s">
         <v>80</v>
       </c>
@@ -4364,7 +4399,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="28">
       <c r="A76" s="5" t="s">
         <v>85</v>
       </c>
@@ -4375,7 +4410,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="56">
       <c r="A77" s="5" t="s">
         <v>82</v>
       </c>
@@ -4386,7 +4421,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="70">
       <c r="A78" s="5" t="s">
         <v>87</v>
       </c>
@@ -4397,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="14">
       <c r="A79" s="5" t="s">
         <v>113</v>
       </c>
@@ -4408,7 +4443,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="14">
       <c r="A80" s="5" t="s">
         <v>115</v>
       </c>
@@ -4419,7 +4454,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="28">
       <c r="A81" s="5" t="s">
         <v>124</v>
       </c>
@@ -4430,7 +4465,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="28">
       <c r="A82" s="11" t="s">
         <v>125</v>
       </c>
@@ -4441,7 +4476,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="28">
       <c r="A83" s="11" t="s">
         <v>126</v>
       </c>
@@ -4452,7 +4487,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="28">
       <c r="A84" s="11" t="s">
         <v>127</v>
       </c>
@@ -4463,7 +4498,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="14">
       <c r="A85" s="5" t="s">
         <v>529</v>
       </c>
@@ -4474,7 +4509,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="14">
       <c r="A86" s="5" t="s">
         <v>531</v>
       </c>
@@ -4485,7 +4520,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="14">
       <c r="A87" s="5" t="s">
         <v>15</v>
       </c>
@@ -4496,7 +4531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="14">
       <c r="A88" s="5" t="s">
         <v>17</v>
       </c>
@@ -4507,7 +4542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="14">
       <c r="A89" s="5" t="s">
         <v>523</v>
       </c>
@@ -4518,7 +4553,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="14">
       <c r="A90" s="5" t="s">
         <v>525</v>
       </c>
@@ -4529,7 +4564,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="28">
       <c r="A91" s="5" t="s">
         <v>519</v>
       </c>
@@ -4540,7 +4575,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="28">
       <c r="A92" s="5" t="s">
         <v>521</v>
       </c>
@@ -4551,7 +4586,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="28">
       <c r="A93" s="5" t="s">
         <v>515</v>
       </c>
@@ -4562,7 +4597,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="28">
       <c r="A94" s="5" t="s">
         <v>517</v>
       </c>
@@ -4573,7 +4608,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="28">
       <c r="A95" s="5" t="s">
         <v>35</v>
       </c>
@@ -4584,7 +4619,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="28">
       <c r="A96" s="5" t="s">
         <v>37</v>
       </c>
@@ -4595,7 +4630,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="28">
       <c r="A97" s="5" t="s">
         <v>29</v>
       </c>
@@ -4606,7 +4641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="28">
       <c r="A98" s="5" t="s">
         <v>27</v>
       </c>
@@ -4617,7 +4652,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="28">
       <c r="A99" s="5" t="s">
         <v>495</v>
       </c>
@@ -4628,7 +4663,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="28">
       <c r="A100" s="5" t="s">
         <v>537</v>
       </c>
@@ -4639,7 +4674,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="28">
       <c r="A101" s="11" t="s">
         <v>128</v>
       </c>
@@ -4650,7 +4685,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="28">
       <c r="A102" s="11" t="s">
         <v>129</v>
       </c>
@@ -4661,7 +4696,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="28">
       <c r="A103" s="11" t="s">
         <v>130</v>
       </c>
@@ -4672,7 +4707,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="28">
       <c r="A104" s="11" t="s">
         <v>131</v>
       </c>
@@ -4683,7 +4718,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="28">
       <c r="A105" s="11" t="s">
         <v>132</v>
       </c>
@@ -4694,7 +4729,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="28">
       <c r="A106" s="11" t="s">
         <v>133</v>
       </c>
@@ -4705,7 +4740,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="28">
       <c r="A107" s="11" t="s">
         <v>134</v>
       </c>
@@ -4716,7 +4751,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="28">
       <c r="A108" s="11" t="s">
         <v>135</v>
       </c>
@@ -4727,7 +4762,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="28">
       <c r="A109" s="11" t="s">
         <v>136</v>
       </c>
@@ -4738,7 +4773,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="14">
       <c r="A110" s="5" t="s">
         <v>71</v>
       </c>
@@ -4749,7 +4784,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="14">
       <c r="A111" s="5" t="s">
         <v>72</v>
       </c>
@@ -4760,7 +4795,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="14">
       <c r="A112" s="5" t="s">
         <v>94</v>
       </c>
@@ -4771,7 +4806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="28">
       <c r="A113" s="5" t="s">
         <v>95</v>
       </c>
@@ -4782,7 +4817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" ht="14">
       <c r="A114" s="5" t="s">
         <v>68</v>
       </c>
@@ -4793,7 +4828,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="28">
       <c r="A115" s="5" t="s">
         <v>69</v>
       </c>
@@ -4804,7 +4839,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="28">
       <c r="A116" s="5" t="s">
         <v>66</v>
       </c>
@@ -4815,7 +4850,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="28">
       <c r="A117" s="5" t="s">
         <v>67</v>
       </c>
@@ -4826,7 +4861,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="28">
       <c r="A118" s="5" t="s">
         <v>64</v>
       </c>
@@ -4837,7 +4872,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="28">
       <c r="A119" s="5" t="s">
         <v>65</v>
       </c>
@@ -4848,7 +4883,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" ht="28">
       <c r="A120" s="5" t="s">
         <v>104</v>
       </c>
@@ -4859,7 +4894,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" ht="28">
       <c r="A121" s="5" t="s">
         <v>105</v>
       </c>
@@ -4870,7 +4905,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" ht="28">
       <c r="A122" s="5" t="s">
         <v>101</v>
       </c>
@@ -4881,7 +4916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" ht="28">
       <c r="A123" s="5" t="s">
         <v>100</v>
       </c>
@@ -4892,7 +4927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="28">
       <c r="A124" s="5" t="s">
         <v>53</v>
       </c>
@@ -4903,7 +4938,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" ht="28">
       <c r="A125" s="5" t="s">
         <v>77</v>
       </c>
@@ -4914,7 +4949,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" ht="28">
       <c r="A126" s="11" t="s">
         <v>146</v>
       </c>
@@ -4925,7 +4960,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" ht="28">
       <c r="A127" s="11" t="s">
         <v>147</v>
       </c>
@@ -4936,7 +4971,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" ht="28">
       <c r="A128" s="11" t="s">
         <v>148</v>
       </c>
@@ -4947,7 +4982,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" ht="28">
       <c r="A129" s="11" t="s">
         <v>149</v>
       </c>
@@ -4958,7 +4993,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" ht="28">
       <c r="A130" s="11" t="s">
         <v>150</v>
       </c>
@@ -4969,7 +5004,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="28">
       <c r="A131" s="11" t="s">
         <v>151</v>
       </c>
@@ -4980,7 +5015,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="28">
       <c r="A132" s="11" t="s">
         <v>152</v>
       </c>
@@ -4991,7 +5026,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" ht="28">
       <c r="A133" s="11" t="s">
         <v>153</v>
       </c>
@@ -5002,7 +5037,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="28">
       <c r="A134" s="11" t="s">
         <v>154</v>
       </c>
@@ -5022,7 +5057,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor indexed="57"/>
   </sheetPr>
@@ -5033,14 +5068,14 @@
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="24" style="3" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14">
       <c r="A1" s="2" t="s">
         <v>291</v>
       </c>
@@ -5051,7 +5086,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="42">
       <c r="A2" s="13" t="s">
         <v>304</v>
       </c>
@@ -5062,7 +5097,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="28">
       <c r="A3" s="13" t="s">
         <v>316</v>
       </c>
@@ -5073,7 +5108,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="42">
       <c r="A4" s="13" t="s">
         <v>155</v>
       </c>
@@ -5084,7 +5119,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="154">
       <c r="A5" s="17" t="s">
         <v>435</v>
       </c>

</xml_diff>